<commit_message>
Update Readme. Add Example Codes.
</commit_message>
<xml_diff>
--- a/examples/EmployeeSalesSummary.xlsx
+++ b/examples/EmployeeSalesSummary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud-sdk-python\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud-sdk-python\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3DBB324-28A0-45C3-926B-3E2529CFC5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596B87A2-33C4-4F85-B0E9-E30A39110A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB5B722-5C7B-460F-9F6A-FDF2D63F0853}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -179,63 +179,60 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,45 +732,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="925" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                    <a:cs typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sales</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0"/>
-              <c:y val="0.52275258478081055"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
@@ -909,14 +867,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -1208,239 +1166,244 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2D5B61-483D-43C7-9020-D1F0B5951987}">
   <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="1.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="1.28515625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="4" style="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" style="13" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="1.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="1.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2">
+      <c r="B2" s="13">
         <v>2003</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="6">
         <v>12</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="8">
+      <c r="B26" s="14">
         <v>2023</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="15" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="6">
         <v>12</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="1" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="17" t="s">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="9" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="18">
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="8">
         <v>944.19600000000003</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="9" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="18">
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="8">
         <v>954.75</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="9" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="18">
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="8">
         <v>2564.0819999999999</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="9" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="18">
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="8">
         <v>23105.466</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="18">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="8">
         <v>27568.493999999999</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="9" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="18">
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="8">
         <v>3589.7939999999999</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="18">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="8">
         <v>3589.7939999999999</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="18">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="8">
         <v>31158.288</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:K28"/>
     <mergeCell ref="B35:K35"/>
     <mergeCell ref="B36:K36"/>
     <mergeCell ref="B29:E32"/>
@@ -1451,16 +1414,11 @@
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="F34:K34"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:K28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1479,42 +1437,42 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>954.75</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="4">
         <v>26695.26</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="4">
         <v>944.19600000000003</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="4">
         <v>2564.0819999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update EmployeeSalesSummary.xlsx and example code for convert apis.
</commit_message>
<xml_diff>
--- a/examples/EmployeeSalesSummary.xlsx
+++ b/examples/EmployeeSalesSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29221"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud-sdk-python\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596B87A2-33C4-4F85-B0E9-E30A39110A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1C149-AFB3-4269-B934-0D860803BEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB5B722-5C7B-460F-9F6A-FDF2D63F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DDB5B722-5C7B-460F-9F6A-FDF2D63F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -173,28 +173,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -207,6 +302,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -219,26 +329,173 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="41"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -432,25 +689,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{5AF9D5C5-FB60-45D0-9B7A-1F68D83B6699}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumn" dxfId="19"/>
+      <tableStyleElement type="lastColumn" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{DC245C9D-BD39-419D-B58B-B23DA8D5365F}">
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
-    </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{DC245C9D-BD39-419D-B58B-B23DA8D5365F}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="10"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="9"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="8"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="7"/>
+      <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -467,7 +724,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -906,6 +1163,17 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{82CC9C96-6988-4556-AE1E-7FD88B72DB7F}" name="Table1" displayName="Table1" ref="C3:D7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="C3:D7" xr:uid="{82CC9C96-6988-4556-AE1E-7FD88B72DB7F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{085C32C4-8C23-43EC-B415-7FC0867F2F66}" name="Product Category" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{71F063F0-6B4C-4D98-9EDC-6CF1C538D4A7}" name="Sales" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1166,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2D5B61-483D-43C7-9020-D1F0B5951987}">
   <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,17 +1455,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="13">
+      <c r="B2" s="6">
         <v>2003</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="3">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -1205,205 +1473,201 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="14">
+      <c r="B26" s="7">
         <v>2023</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="5" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="3">
         <v>12</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17" t="s">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
       <c r="K28" s="17"/>
-      <c r="L28" s="7" t="s">
+      <c r="L28" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12" t="s">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="8">
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="5">
         <v>944.19600000000003</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12" t="s">
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="8">
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="5">
         <v>954.75</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12" t="s">
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="8">
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="5">
         <v>2564.0819999999999</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="8">
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="5">
         <v>23105.466</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="8">
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="5">
         <v>27568.493999999999</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12" t="s">
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="8">
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="5">
         <v>3589.7939999999999</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="8">
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="5">
         <v>3589.7939999999999</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="8">
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="5">
         <v>31158.288</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="F28:K28"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:K28"/>
     <mergeCell ref="B35:K35"/>
     <mergeCell ref="B36:K36"/>
     <mergeCell ref="B29:E32"/>
@@ -1414,6 +1678,10 @@
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="F34:K34"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="J26:L26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1426,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA87F232-935F-44EE-BD47-3596F793DF44}">
   <dimension ref="C3:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1437,47 +1705,50 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="41" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="38">
         <v>954.75</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="38">
         <v>26695.26</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="38">
         <v>944.19600000000003</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="39">
         <v>2564.0819999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>